<commit_message>
Committing changes for phs002504
</commit_message>
<xml_diff>
--- a/InputFiles/CCDI/TC01_CCDI_phs002504_Sex-Female.xlsx
+++ b/InputFiles/CCDI/TC01_CCDI_phs002504_Sex-Female.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sohilz2/Automation/poc-09-25-2024/Commons_Automation/InputFiles/CCDI/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tatekaraa\Automation\12-16-24\Commons_Automation\InputFiles\CCDI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5042468-9A56-0045-B7AF-60AC9A4EEF84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB6B422B-AE4A-49E4-9CD6-B214BFB5AD9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30240" yWindow="-4180" windowWidth="51200" windowHeight="28800" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -68,150 +68,194 @@
     <t>StudiesTab</t>
   </si>
   <si>
+    <t xml:space="preserve">SELECT
+    std.study_name AS "Study Name",
+    std.study AS "Study ID",
+    CONCAT(dgn.diagnosis, ' (', COUNT(DISTINCT dgn.diagnosis_id), ')') AS "Diagnosis (Top 5)",
+    dgn.anatomic_site AS "Diagnosis Anatomic Site (Top 5)",
+    COUNT(DISTINCT prt.participant_id) AS "Number of Participants"
+FROM 
+    df_study std
+LEFT JOIN 
+    df_participant prt ON std.id = prt."study.id"
+LEFT JOIN 
+    df_diagnosis dgn ON prt.id = dgn."participant.id"
+LEFT JOIN 
+    df_publication pub ON std.id = pub."study.id"
+WHERE 
+    std.study = 'phs002504' AND prt.sex_at_birth IN ('Male', 'Female', 'Unknown')
+</t>
+  </si>
+  <si>
+    <t>SELECT DISTINCT
+    prt.participant_id AS "Participant ID",
+    std.study AS "Study ID",
+    COALESCE(prt.sex_at_birth, '') AS "Sex",
+    COALESCE(prt.race, '') AS "Race",
+    COALESCE(CAST(syn.synonym_id AS INT), '') AS "Synonym Participant ID"
+FROM 
+    df_study std
+LEFT JOIN 
+    df_participant prt ON std.id = prt."study.id"
+LEFT JOIN 
+    df_sample smp ON prt.id = smp."participant.id"
+LEFT JOIN 
+    df_diagnosis dgn ON prt.id = dgn."participant.id"
+LEFT JOIN 
+    df_publication pub ON std.id = pub."study.id"
+LEFT JOIN 
+    df_follow_up flw ON prt.id = flw."participant.id"
+LEFT JOIN 
+    df_sequencing_file seq ON smp.id = seq."sample.id"
+LEFT JOIN 
+    df_study_admin adm ON std.id = adm."study.id"
+LEFT JOIN 
+    df_study_personnel per ON std.id = per."study.id"
+LEFT JOIN 
+    df_study_funding fund ON std.id = fund."study.id"
+LEFT JOIN 
+    df_methylation_array_file maf ON smp.id = maf."sample.id"
+LEFT JOIN 
+    df_synonym syn ON prt.id = syn."participant.id"
+LEFT JOIN 
+    df_treatment trt ON prt.id = trt."participant.id"
+LEFT JOIN 
+    df_treatment_resp trr ON prt.id = trr."participant.id"
+WHERE 
+    std.study = 'phs002504' AND prt.sex_at_birth = 'Female'
+ORDER BY 
+    prt.participant_id ASC
+LIMIT 100;</t>
+  </si>
+  <si>
     <t>SELECT
-    p.participant_id AS "Participant ID",
-    st.study_id AS "Study ID",
-    COALESCE(p.sex_at_birth, '') AS "Sex",
-    COALESCE(p.race, '') AS "Race",
-    COALESCE(p.ethnicity, '') AS "Ethnicity",
-    COALESCE(CAST(p.alternate_participant_id AS INT), '') AS "Alternate ID"
+    COUNT(DISTINCT std.study) AS "Studies",
+    COUNT(DISTINCT prt.participant_id) AS "Participants",
+    COUNT(DISTINCT smp.sample_id) AS "Samples",
+    (COUNT(DISTINCT seq.id) + COUNT(DISTINCT maf.id)) AS "Files"
 FROM 
-    df_participant p
-JOIN 
-    df_study st ON p."study.id" = st.id
-LEFT JOIN 
-    df_sample smp ON smp."participant.id" = p.participant_id
-LEFT JOIN 
-    df_diagnosis diag ON diag."participant.id" = p.participant_id
-LEFT JOIN 
-    df_publication pub ON pub."study.id" = st.study_id
-LEFT JOIN 
-    df_sequencing_file sqf ON sqf."sample.id" = smp.sample_id
+    df_study std
+LEFT JOIN 
+    df_participant prt ON std.id = prt."study.id"
+LEFT JOIN 
+    df_sample smp ON prt.id = smp."participant.id"
+LEFT JOIN 
+    df_diagnosis dgn ON prt.id = dgn."participant.id"
+LEFT JOIN 
+    df_publication pub ON std.id = pub."study.id"
+LEFT JOIN 
+    df_follow_up flw ON prt.id = flw."participant.id"
+LEFT JOIN 
+    df_sequencing_file seq ON smp.id = seq."sample.id"
+LEFT JOIN 
+    df_study_admin adm ON std.id = adm."study.id"
+LEFT JOIN 
+    df_study_personnel per ON std.id = per."study.id"
+LEFT JOIN 
+    df_study_funding fund ON std.id = fund."study.id"
+LEFT JOIN 
+    df_methylation_array_file maf ON smp.id = maf."sample.id"
+LEFT JOIN 
+    df_synonym syn ON prt.id = syn."participant.id"
+LEFT JOIN 
+    df_treatment trt ON prt.id = trt."participant.id"
+LEFT JOIN 
+    df_treatment_resp trr ON prt.id = trr."participant.id"
 WHERE 
-    st.study_id = 'phs002504' AND p.sex_at_birth = 'Female'
+    std.study = 'phs002504' AND prt.sex_at_birth = 'Female';</t>
+  </si>
+  <si>
+    <t>TC01_CCDI_phs002504_Sex-Female_TSVData.xlsx</t>
+  </si>
+  <si>
+    <t>TC01_CCDI_phs002504_Sex-Female_WebData.xlsx</t>
+  </si>
+  <si>
+    <t>SELECT DISTINCT
+    prt.participant_id AS "Participant ID",
+    COALESCE(smp.sample_id, '') AS "Sample ID",
+    std.study AS "Study ID",
+    COALESCE(dgn.diagnosis, '') AS "Diagnosis",
+    COALESCE(dgn.anatomic_site, '') AS "Diagnosis Anatomic Site",
+    COALESCE(dgn.diagnosis_classification_system, '') AS "Diagnosis Classification System",
+    COALESCE(dgn.diagnosis_basis, '') AS "Diagnosis Basis",    
+    COALESCE(dgn.disease_phase, '') AS "Disease Phase",
+    COALESCE(CASE WHEN dgn.age_at_diagnosis = -999 THEN 'Not Reported' ELSE dgn.age_at_diagnosis END, 0) AS "Age at Diagnosis (days)",
+    COALESCE(srv.last_known_survival_status, '') AS "Last Known Survival Status"
+FROM 
+    df_study std
+LEFT JOIN 
+    df_participant prt ON std.id = prt."study.id"
+LEFT JOIN 
+    df_sample smp ON prt.id = smp."participant.id"
+LEFT JOIN 
+    df_diagnosis dgn ON prt.id = dgn."participant.id"
+LEFT JOIN 
+    df_publication pub ON std.id = pub."study.id"
+LEFT JOIN 
+    df_follow_up flw ON prt.id = flw."participant.id"
+LEFT JOIN 
+    df_sequencing_file seq ON smp.id = seq."sample.id"
+LEFT JOIN 
+    df_study_admin adm ON std.id = adm."study.id"
+LEFT JOIN 
+    df_study_personnel per ON std.id = per."study.id"
+LEFT JOIN 
+    df_study_funding fund ON std.id = fund."study.id"
+LEFT JOIN 
+    df_methylation_array_file maf ON smp.id = maf."sample.id"
+LEFT JOIN 
+    df_synonym syn ON prt.id = syn."participant.id"
+LEFT JOIN 
+    df_treatment trt ON prt.id = trt."participant.id"
+LEFT JOIN 
+    df_treatment_resp trr ON prt.id = trr."participant.id"
+LEFT JOIN 
+    df_survival srv ON prt.id = srv."participant.id"
+WHERE 
+    std.study = 'phs002504' AND prt.sex_at_birth = 'Female'
 ORDER BY 
-    p.participant_id ASC
-LIMIT 100;</t>
-  </si>
-  <si>
-    <t>SELECT
-    COUNT(DISTINCT st.study_id) AS "Studies",
-    COUNT(DISTINCT p.participant_id) AS "Participants",
-    COUNT(DISTINCT smp.sample_id) AS "Samples",
-    COUNT(DISTINCT sf.id) AS "Files"
-FROM 
-    df_participant p
-JOIN 
-    df_study st ON p."study.id" = st.id
-LEFT JOIN 
-    df_sample smp ON smp."participant.id" = p.id
-LEFT JOIN 
-    df_sequencing_file sf ON sf."sample.id" = smp.id
-LEFT JOIN 
-    df_methylation_array_file maf ON maf."sample.id" = smp.sample_id
-WHERE 
-    st.study_id = 'phs002504' AND p.sex_at_birth = 'Female';</t>
-  </si>
-  <si>
-    <t>TC01_CCDI_phs002504_Sex-Female_TSVData.xlsx</t>
-  </si>
-  <si>
-    <t>TC01_CCDI_phs002504_Sex-Female_WebData.xlsx</t>
-  </si>
-  <si>
-    <t>SELECT
-    p.participant_id AS "Participant ID",
-    st.study_id AS "Study ID",
-    COALESCE(diag.diagnosis_classification, '') AS "Diagnosis",
-    COALESCE(diag.anatomic_site, '') AS "Diagnosis Anatomic Site",
-    COALESCE(diag.diagnosis_classification_system, '') AS "Diagnosis Classification System",
-    COALESCE(diag.diagnosis_verification_status, '') AS "Diagnosis Verification Status",
-    COALESCE(diag.diagnosis_basis, '') AS "Diagnosis Basis",
-    COALESCE(diag.diagnosis_comment, '') AS "Diagnosis Comment",
-    COALESCE(diag.disease_phase, '') AS "Disease Phase",
-    COALESCE(CASE WHEN diag.age_at_diagnosis = -999 THEN 'Not Reported' ELSE diag.age_at_diagnosis END, 0) AS "Age at Diagnosis (days)",
-    COALESCE(fu.vital_status, '') AS "Vital Status"
-FROM 
-    df_participant p
-JOIN 
-    df_study st ON p."study.id" = st.id
-LEFT JOIN 
-    df_diagnosis diag ON diag."participant.id" = p.id
-LEFT JOIN 
-    df_follow_up fu ON fu."participant.id" = p.id
-WHERE 
-    st.study_id = 'phs002504' AND p.sex_at_birth = 'Female'
-ORDER BY 
-    p.participant_id ASC
-LIMIT 100;</t>
-  </si>
-  <si>
-    <t>SELECT
-    st.study_short_title AS "Study Short Title",
-    st.study_id AS "Study ID",
-    diag.diagnosis_classification AS "Diagnosis (Top 5)",
-    COUNT(diag.anatomic_site) AS "Diagnosis Anatomic Site (Top 5)",
-    COUNT(DISTINCT p.participant_id) AS "Number of Participants",
-    COUNT(DISTINCT smp.sample_id) AS "Number of Samples",
-    COUNT(DISTINCT sqf.sequencing_file_id) AS "Number of Files",
-    GROUP_CONCAT(DISTINCT sqf.file_type) AS "File Type (Top 5)",
-    GROUP_CONCAT(DISTINCT pub.pubmed_id) AS "PubMed ID",
-    sp.personnel_name AS "Principal Investigator(s)",
-    sf.grant_id AS "Grant ID"
-FROM 
-    df_study st
-JOIN 
-    df_participant p ON p."study.id" = st.id
-LEFT JOIN 
-    df_sample smp ON smp."participant.id" = p.participant_id
-LEFT JOIN 
-    df_diagnosis diag ON diag."participant.id" = p.participant_id
-LEFT JOIN 
-    df_publication pub ON pub."study.id" = st.study_id
-LEFT JOIN 
-    df_sequencing_file sqf ON sqf."sample.id" = smp.sample_id
-LEFT JOIN 
-    df_study_personnel sp ON sp."study.id" = st.study_id
-LEFT JOIN 
-    df_study_funding sf ON sf."study.id" = st.study_id
-WHERE 
-    st.study_id = 'phs002504' AND p.sex_at_birth = 'Female'
-GROUP BY 
-    st.study_short_title, st.study_id, sf.grant_id
-ORDER BY 
-    st.study_id ASC
-LIMIT 100;</t>
+    prt.participant_id ASC;</t>
   </si>
   <si>
     <t>SELECT DISTINCT
     smp.sample_id AS "Sample ID",
-    p.participant_id AS "Participant ID",
-    st.study_id AS "Study ID",
+    prt.participant_id AS "Participant ID",
+    std.study AS "Study ID",
     smp.anatomic_site AS "Sample Anatomic Site",
     COALESCE(CASE WHEN smp.participant_age_at_collection = -999 THEN 'Not Reported' ELSE smp.participant_age_at_collection END, 0) AS "Age at Sample Collection (days)",
-    COALESCE(diag.diagnosis_classification, '') AS "Diagnosis",
-    COALESCE(diag.diagnosis_classification_system, '') AS "Diagnosis Classification System",
-    COALESCE(diag.diagnosis_verification_status, '') AS "Diagnosis Verification Status",
-    COALESCE(diag.diagnosis_basis, '') AS "Diagnosis Basis",
-    COALESCE(diag.diagnosis_comment, '') AS "Diagnosis Comment",
     COALESCE(smp.sample_tumor_status, '') AS "Sample Tumor Status",
     COALESCE(smp.tumor_classification, '') AS "Sample Tumor Classification"
 FROM 
-    df_participant p
-JOIN 
-    df_study st ON p."study.id" = st.id
-LEFT JOIN 
-    df_sample smp ON smp."participant.id" = p.id
-LEFT JOIN 
-    df_diagnosis diag ON diag."participant.id" = p.id
-LEFT JOIN 
-    df_follow_up fu ON fu."participant.id" = p.id
-LEFT JOIN 
-    df_publication pub ON pub."study.id" = st.study_id
-LEFT JOIN 
-    df_sequencing_file sqf ON sqf."sample.id" = smp.sample_id
+    df_study std
+LEFT JOIN 
+    df_participant prt ON std.id = prt."study.id"
+LEFT JOIN 
+    df_sample smp ON prt.id = smp."participant.id"
+LEFT JOIN 
+    df_diagnosis dgn ON prt.id = dgn."participant.id"
+LEFT JOIN 
+    df_publication pub ON std.id = pub."study.id"
+LEFT JOIN 
+    df_follow_up flw ON prt.id = flw."participant.id"
+LEFT JOIN 
+    df_sequencing_file seq ON smp.id = seq."sample.id"
+LEFT JOIN 
+    df_study_admin adm ON std.id = adm."study.id"
+LEFT JOIN 
+    df_study_personnel per ON std.id = per."study.id"
+LEFT JOIN 
+    df_study_funding fund ON std.id = fund."study.id"
+LEFT JOIN 
+    df_methylation_array_file maf ON smp.id = maf."sample.id"
+LEFT JOIN 
+    df_synonym syn ON prt.id = syn."participant.id"
+LEFT JOIN 
+    df_treatment trt ON prt.id = trt."participant.id"
+LEFT JOIN 
+    df_treatment_resp trr ON prt.id = trr."participant.id"
 WHERE 
-    st.study_id = 'phs002504' AND p.sex_at_birth = 'Female' AND smp.sample_id IS NOT NULL
+    std.study = 'phs002504' AND prt.sex_at_birth = 'Female' AND smp.sample_id IS NOT NULL
 ORDER BY 
     smp.sample_id ASC
 LIMIT 100;</t>
@@ -301,30 +345,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -384,23 +407,14 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -726,19 +740,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="C2" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="75.83203125" customWidth="1"/>
-    <col min="4" max="4" width="70.1640625" customWidth="1"/>
-    <col min="5" max="5" width="63.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="75.85546875" customWidth="1"/>
+    <col min="4" max="4" width="70.140625" customWidth="1"/>
+    <col min="5" max="5" width="63.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -755,68 +769,68 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="404" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="6" t="s">
         <v>11</v>
       </c>
+      <c r="C2" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C3" s="3"/>
     </row>
-    <row r="4" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="299.25" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C4" s="3"/>
     </row>
-    <row r="5" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C8" s="1"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>